<commit_message>
Completed create new patient
</commit_message>
<xml_diff>
--- a/OpenEMR New Patient/Default.xlsx
+++ b/OpenEMR New Patient/Default.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
     <sheet name="OpenEMR_Launch_URL" sheetId="2" r:id="rId2"/>
     <sheet name="OpenEMR_Practice_Login" sheetId="3" r:id="rId3"/>
     <sheet name="OpenEMR_Add_New_Patient" sheetId="4" r:id="rId4"/>
+    <sheet name="OpenEMR_Practice_Logoff" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -526,6 +527,25 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>

</xml_diff>

<commit_message>
Updated so that the warning color on the application after filling out the value is no longer shown.  Changed to use the Name: label as an anchor for the three name fields.
</commit_message>
<xml_diff>
--- a/OpenEMR New Patient/Default.xlsx
+++ b/OpenEMR New Patient/Default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -12,9 +12,24 @@
     <sheet name="OpenEMR_Practice_Login" sheetId="3" r:id="rId3"/>
     <sheet name="OpenEMR_Add_New_Patient" sheetId="4" r:id="rId4"/>
     <sheet name="OpenEMR_Practice_Logoff" sheetId="5" r:id="rId5"/>
+    <sheet name="OpenEMR_Patient_Portal_Firs..00" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+  <si>
+    <t>NewPatientPassword</t>
+  </si>
+  <si>
+    <t>NewPatientLogin</t>
+  </si>
+  <si>
+    <t>NewPatientEmail</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -157,7 +172,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -165,15 +180,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,16 +508,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.23046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.74609375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.3671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customFormat="1"/>
+    <row r="1" ht="14.95" s="3" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -493,12 +544,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -517,7 +568,7 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -536,13 +587,32 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -555,7 +625,7 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>